<commit_message>
Financial summary working!  Trying it out right now at /financialSummaryTest.  Five variables are holding unexpected results.  Debugging now.
</commit_message>
<xml_diff>
--- a/db/Book1.xlsx
+++ b/db/Book1.xlsx
@@ -24,70 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="117">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>user_id</t>
-  </si>
-  <si>
-    <t>restaurant_id</t>
-  </si>
-  <si>
-    <t>shiftDate</t>
-  </si>
-  <si>
-    <t>timeIn</t>
-  </si>
-  <si>
-    <t>timeOut</t>
-  </si>
-  <si>
-    <t>shiftType</t>
-  </si>
-  <si>
-    <t>largestTip</t>
-  </si>
-  <si>
-    <t>smallestTip</t>
-  </si>
-  <si>
-    <t>stiffed</t>
-  </si>
-  <si>
-    <t>bwl</t>
-  </si>
-  <si>
-    <t>sales</t>
-  </si>
-  <si>
-    <t>tipout</t>
-  </si>
-  <si>
-    <t>totalWalkedWith</t>
-  </si>
-  <si>
-    <t>tipPercent</t>
-  </si>
-  <si>
-    <t>ppa</t>
-  </si>
-  <si>
-    <t>comments</t>
-  </si>
-  <si>
-    <t>breakthroughs</t>
-  </si>
-  <si>
-    <t>isReal</t>
-  </si>
-  <si>
-    <t>createdAt</t>
-  </si>
-  <si>
-    <t>updatedAt</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="96">
   <si>
     <t>dinner</t>
   </si>
@@ -694,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:U20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -723,73 +660,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="H1">
+        <v>20</v>
+      </c>
+      <c r="I1">
+        <v>4.5</v>
+      </c>
+      <c r="J1">
+        <v>0</v>
+      </c>
+      <c r="K1">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="L1">
+        <v>1234.56</v>
+      </c>
+      <c r="M1">
+        <v>98.76</v>
+      </c>
+      <c r="N1">
+        <v>129.63</v>
+      </c>
+      <c r="O1">
+        <v>18.5</v>
+      </c>
+      <c r="P1">
+        <v>35.450000000000003</v>
       </c>
       <c r="Q1" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="S1">
+        <v>0</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -798,63 +735,63 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>25</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>9.89</v>
+      </c>
+      <c r="L2">
+        <v>654.89</v>
+      </c>
+      <c r="M2">
+        <v>52.39</v>
+      </c>
+      <c r="N2">
+        <v>75.709999999999994</v>
+      </c>
+      <c r="O2">
+        <v>19.559999999999999</v>
+      </c>
+      <c r="P2">
+        <v>42.51</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2">
-        <v>20</v>
-      </c>
-      <c r="I2">
-        <v>4.5</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>8.4499999999999993</v>
-      </c>
-      <c r="L2">
-        <v>1234.56</v>
-      </c>
-      <c r="M2">
-        <v>98.76</v>
-      </c>
-      <c r="N2">
-        <v>129.63</v>
-      </c>
-      <c r="O2">
-        <v>18.5</v>
-      </c>
-      <c r="P2">
-        <v>35.450000000000003</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R2" t="s">
-        <v>42</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="U2" s="1" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -863,63 +800,63 @@
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>22.5</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>10.53</v>
+      </c>
+      <c r="L3">
+        <v>897.85</v>
+      </c>
+      <c r="M3">
+        <v>71.83</v>
+      </c>
+      <c r="N3">
+        <v>108.82</v>
+      </c>
+      <c r="O3">
+        <v>20.12</v>
+      </c>
+      <c r="P3">
+        <v>39.450000000000003</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3">
-        <v>25</v>
-      </c>
-      <c r="I3">
-        <v>5</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>9.89</v>
-      </c>
-      <c r="L3">
-        <v>654.89</v>
-      </c>
-      <c r="M3">
-        <v>52.39</v>
-      </c>
-      <c r="N3">
-        <v>75.709999999999994</v>
-      </c>
-      <c r="O3">
-        <v>19.559999999999999</v>
-      </c>
-      <c r="P3">
-        <v>42.51</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>23</v>
-      </c>
-      <c r="R3" t="s">
-        <v>43</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="U3" s="1" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -928,128 +865,128 @@
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>15.75</v>
+      </c>
+      <c r="I4">
+        <v>3.5</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>12.5</v>
+      </c>
+      <c r="L4">
+        <v>1000</v>
+      </c>
+      <c r="M4">
+        <v>80</v>
+      </c>
+      <c r="N4">
+        <v>98.9</v>
+      </c>
+      <c r="O4">
+        <v>17.89</v>
+      </c>
+      <c r="P4">
+        <v>31.15</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R4" t="s">
+        <v>24</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4">
-        <v>22.5</v>
-      </c>
-      <c r="I4">
-        <v>6</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>10.53</v>
-      </c>
-      <c r="L4">
-        <v>897.85</v>
-      </c>
-      <c r="M4">
-        <v>71.83</v>
-      </c>
-      <c r="N4">
-        <v>108.82</v>
-      </c>
-      <c r="O4">
-        <v>20.12</v>
-      </c>
-      <c r="P4">
-        <v>39.450000000000003</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>24</v>
-      </c>
-      <c r="R4" t="s">
-        <v>44</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="U4" s="1" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>20</v>
+      </c>
+      <c r="I5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>13</v>
+      </c>
+      <c r="L5">
+        <v>1415.23</v>
+      </c>
+      <c r="M5">
+        <v>113.22</v>
+      </c>
+      <c r="N5">
+        <v>147.88999999999999</v>
+      </c>
+      <c r="O5">
+        <v>18.45</v>
+      </c>
+      <c r="P5">
+        <v>56.15</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R5" t="s">
+        <v>25</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5">
-        <v>15.75</v>
-      </c>
-      <c r="I5">
-        <v>3.5</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>12.5</v>
-      </c>
-      <c r="L5">
-        <v>1000</v>
-      </c>
-      <c r="M5">
-        <v>80</v>
-      </c>
-      <c r="N5">
-        <v>98.9</v>
-      </c>
-      <c r="O5">
-        <v>17.89</v>
-      </c>
-      <c r="P5">
-        <v>31.15</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>25</v>
-      </c>
-      <c r="R5" t="s">
-        <v>45</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="U5" s="1" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1058,63 +995,63 @@
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>25</v>
+      </c>
+      <c r="I6">
+        <v>2.75</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>9.56</v>
+      </c>
+      <c r="L6">
+        <v>789.45</v>
+      </c>
+      <c r="M6">
+        <v>63.16</v>
+      </c>
+      <c r="N6">
+        <v>107.05</v>
+      </c>
+      <c r="O6">
+        <v>21.56</v>
+      </c>
+      <c r="P6">
+        <v>38.51</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>6</v>
+      </c>
+      <c r="R6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6">
-        <v>20</v>
-      </c>
-      <c r="I6">
-        <v>4</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>13</v>
-      </c>
-      <c r="L6">
-        <v>1415.23</v>
-      </c>
-      <c r="M6">
-        <v>113.22</v>
-      </c>
-      <c r="N6">
-        <v>147.88999999999999</v>
-      </c>
-      <c r="O6">
-        <v>18.45</v>
-      </c>
-      <c r="P6">
-        <v>56.15</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>26</v>
-      </c>
-      <c r="R6" t="s">
-        <v>46</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="U6" s="1" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1123,63 +1060,63 @@
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>50</v>
+      </c>
+      <c r="I7">
+        <v>6.5</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="L7">
+        <v>654.89</v>
+      </c>
+      <c r="M7">
+        <v>52.39</v>
+      </c>
+      <c r="N7">
+        <v>79.569999999999993</v>
+      </c>
+      <c r="O7">
+        <v>20.149999999999999</v>
+      </c>
+      <c r="P7">
+        <v>39</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>7</v>
+      </c>
+      <c r="R7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7">
-        <v>25</v>
-      </c>
-      <c r="I7">
-        <v>2.75</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>9.56</v>
-      </c>
-      <c r="L7">
-        <v>789.45</v>
-      </c>
-      <c r="M7">
-        <v>63.16</v>
-      </c>
-      <c r="N7">
-        <v>107.05</v>
-      </c>
-      <c r="O7">
-        <v>21.56</v>
-      </c>
-      <c r="P7">
-        <v>38.51</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>27</v>
-      </c>
-      <c r="R7" t="s">
-        <v>47</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="U7" s="1" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1188,63 +1125,63 @@
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>30.56</v>
+      </c>
+      <c r="I8">
+        <v>5.25</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>5.46</v>
+      </c>
+      <c r="L8">
+        <v>894.56</v>
+      </c>
+      <c r="M8">
+        <v>71.56</v>
+      </c>
+      <c r="N8">
+        <v>107.35</v>
+      </c>
+      <c r="O8">
+        <v>20</v>
+      </c>
+      <c r="P8">
+        <v>34.15</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>8</v>
+      </c>
+      <c r="R8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8">
-        <v>50</v>
-      </c>
-      <c r="I8">
-        <v>6.5</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <v>8.4600000000000009</v>
-      </c>
-      <c r="L8">
-        <v>654.89</v>
-      </c>
-      <c r="M8">
-        <v>52.39</v>
-      </c>
-      <c r="N8">
-        <v>79.569999999999993</v>
-      </c>
-      <c r="O8">
-        <v>20.149999999999999</v>
-      </c>
-      <c r="P8">
-        <v>39</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>28</v>
-      </c>
-      <c r="R8" t="s">
-        <v>48</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="U8" s="1" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1253,63 +1190,63 @@
         <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="G9" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>30.56</v>
+        <v>15</v>
       </c>
       <c r="I9">
-        <v>5.25</v>
+        <v>4.25</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9">
-        <v>5.46</v>
+        <v>2.46</v>
       </c>
       <c r="L9">
-        <v>894.56</v>
+        <v>1005</v>
       </c>
       <c r="M9">
-        <v>71.56</v>
+        <v>80.400000000000006</v>
       </c>
       <c r="N9">
-        <v>107.35</v>
+        <v>110.55</v>
       </c>
       <c r="O9">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P9">
-        <v>34.15</v>
+        <v>35.6</v>
       </c>
       <c r="Q9" t="s">
+        <v>9</v>
+      </c>
+      <c r="R9" t="s">
         <v>29</v>
       </c>
-      <c r="R9" t="s">
-        <v>49</v>
-      </c>
       <c r="S9">
         <v>0</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1318,63 +1255,63 @@
         <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="G10" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I10">
-        <v>4.25</v>
+        <v>5.32</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>2.46</v>
+        <v>7.86</v>
       </c>
       <c r="L10">
-        <v>1005</v>
+        <v>1325.15</v>
       </c>
       <c r="M10">
-        <v>80.400000000000006</v>
+        <v>106.01</v>
       </c>
       <c r="N10">
-        <v>110.55</v>
+        <v>154.38</v>
       </c>
       <c r="O10">
-        <v>19</v>
+        <v>19.649999999999999</v>
       </c>
       <c r="P10">
-        <v>35.6</v>
+        <v>40.119999999999997</v>
       </c>
       <c r="Q10" t="s">
+        <v>10</v>
+      </c>
+      <c r="R10" t="s">
         <v>30</v>
       </c>
-      <c r="R10" t="s">
-        <v>50</v>
-      </c>
       <c r="S10">
         <v>0</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1383,63 +1320,63 @@
         <v>0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>18</v>
+        <v>13.56</v>
       </c>
       <c r="I11">
-        <v>5.32</v>
+        <v>4.78</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11">
-        <v>7.86</v>
+        <v>8.49</v>
       </c>
       <c r="L11">
-        <v>1325.15</v>
+        <v>1243.56</v>
       </c>
       <c r="M11">
-        <v>106.01</v>
+        <v>99.48</v>
       </c>
       <c r="N11">
-        <v>154.38</v>
+        <v>125.85</v>
       </c>
       <c r="O11">
-        <v>19.649999999999999</v>
+        <v>18.12</v>
       </c>
       <c r="P11">
-        <v>40.119999999999997</v>
+        <v>45.31</v>
       </c>
       <c r="Q11" t="s">
+        <v>11</v>
+      </c>
+      <c r="R11" t="s">
         <v>31</v>
       </c>
-      <c r="R11" t="s">
-        <v>51</v>
-      </c>
       <c r="S11">
         <v>0</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1448,63 +1385,63 @@
         <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="G12" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>13.56</v>
+        <v>65</v>
       </c>
       <c r="I12">
-        <v>4.78</v>
+        <v>5.5</v>
       </c>
       <c r="J12">
         <v>0</v>
       </c>
       <c r="K12">
-        <v>8.49</v>
+        <v>3.49</v>
       </c>
       <c r="L12">
-        <v>1243.56</v>
+        <v>765.48</v>
       </c>
       <c r="M12">
-        <v>99.48</v>
+        <v>61.24</v>
       </c>
       <c r="N12">
-        <v>125.85</v>
+        <v>72.180000000000007</v>
       </c>
       <c r="O12">
-        <v>18.12</v>
+        <v>17.43</v>
       </c>
       <c r="P12">
-        <v>45.31</v>
+        <v>49.76</v>
       </c>
       <c r="Q12" t="s">
+        <v>12</v>
+      </c>
+      <c r="R12" t="s">
         <v>32</v>
       </c>
-      <c r="R12" t="s">
-        <v>52</v>
-      </c>
       <c r="S12">
         <v>0</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1513,63 +1450,63 @@
         <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="G13" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H13">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="I13">
-        <v>5.5</v>
+        <v>2.5</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
       <c r="K13">
-        <v>3.49</v>
+        <v>10.56</v>
       </c>
       <c r="L13">
-        <v>765.48</v>
+        <v>485.15</v>
       </c>
       <c r="M13">
-        <v>61.24</v>
+        <v>38.81</v>
       </c>
       <c r="N13">
-        <v>72.180000000000007</v>
+        <v>39.44</v>
       </c>
       <c r="O13">
-        <v>17.43</v>
+        <v>16.13</v>
       </c>
       <c r="P13">
-        <v>49.76</v>
+        <v>51.45</v>
       </c>
       <c r="Q13" t="s">
+        <v>13</v>
+      </c>
+      <c r="R13" t="s">
         <v>33</v>
       </c>
-      <c r="R13" t="s">
-        <v>53</v>
-      </c>
       <c r="S13">
         <v>0</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1578,63 +1515,63 @@
         <v>0</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="G14" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <v>42</v>
+        <v>32.15</v>
       </c>
       <c r="I14">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="J14">
         <v>0</v>
       </c>
       <c r="K14">
-        <v>10.56</v>
+        <v>12</v>
       </c>
       <c r="L14">
-        <v>485.15</v>
+        <v>598.55999999999995</v>
       </c>
       <c r="M14">
-        <v>38.81</v>
+        <v>47.88</v>
       </c>
       <c r="N14">
-        <v>39.44</v>
+        <v>68.540000000000006</v>
       </c>
       <c r="O14">
-        <v>16.13</v>
+        <v>19.45</v>
       </c>
       <c r="P14">
-        <v>51.45</v>
+        <v>29.46</v>
       </c>
       <c r="Q14" t="s">
+        <v>14</v>
+      </c>
+      <c r="R14" t="s">
         <v>34</v>
       </c>
-      <c r="R14" t="s">
-        <v>54</v>
-      </c>
       <c r="S14">
         <v>0</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1643,63 +1580,63 @@
         <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="G15" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H15">
-        <v>32.15</v>
+        <v>20</v>
       </c>
       <c r="I15">
-        <v>3.5</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="J15">
         <v>0</v>
       </c>
       <c r="K15">
-        <v>12</v>
+        <v>14.45</v>
       </c>
       <c r="L15">
-        <v>598.55999999999995</v>
+        <v>984.56</v>
       </c>
       <c r="M15">
-        <v>47.88</v>
+        <v>79</v>
       </c>
       <c r="N15">
-        <v>68.540000000000006</v>
+        <v>114.85</v>
       </c>
       <c r="O15">
-        <v>19.45</v>
+        <v>19.63</v>
       </c>
       <c r="P15">
-        <v>29.46</v>
+        <v>34.15</v>
       </c>
       <c r="Q15" t="s">
+        <v>15</v>
+      </c>
+      <c r="R15" t="s">
         <v>35</v>
       </c>
-      <c r="R15" t="s">
-        <v>55</v>
-      </c>
       <c r="S15">
         <v>0</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1708,63 +1645,63 @@
         <v>0</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="G16" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H16">
-        <v>20</v>
+        <v>15.5</v>
       </c>
       <c r="I16">
-        <v>4.6500000000000004</v>
+        <v>5</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
       <c r="K16">
-        <v>14.45</v>
+        <v>15.56</v>
       </c>
       <c r="L16">
-        <v>984.56</v>
+        <v>1023.56</v>
       </c>
       <c r="M16">
-        <v>79</v>
+        <v>81.88</v>
       </c>
       <c r="N16">
-        <v>114.85</v>
+        <v>106.97</v>
       </c>
       <c r="O16">
-        <v>19.63</v>
+        <v>18.45</v>
       </c>
       <c r="P16">
-        <v>34.15</v>
+        <v>35</v>
       </c>
       <c r="Q16" t="s">
+        <v>16</v>
+      </c>
+      <c r="R16" t="s">
         <v>36</v>
       </c>
-      <c r="R16" t="s">
-        <v>56</v>
-      </c>
       <c r="S16">
         <v>0</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1773,63 +1710,63 @@
         <v>0</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="G17" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>15.5</v>
+        <v>10.5</v>
       </c>
       <c r="I17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J17">
         <v>0</v>
       </c>
       <c r="K17">
-        <v>15.56</v>
+        <v>13.2</v>
       </c>
       <c r="L17">
-        <v>1023.56</v>
+        <v>948.56</v>
       </c>
       <c r="M17">
-        <v>81.88</v>
+        <v>75.88</v>
       </c>
       <c r="N17">
-        <v>106.97</v>
+        <v>90.69</v>
       </c>
       <c r="O17">
-        <v>18.45</v>
+        <v>17.559999999999999</v>
       </c>
       <c r="P17">
-        <v>35</v>
+        <v>35.159999999999997</v>
       </c>
       <c r="Q17" t="s">
+        <v>17</v>
+      </c>
+      <c r="R17" t="s">
         <v>37</v>
       </c>
-      <c r="R17" t="s">
-        <v>57</v>
-      </c>
       <c r="S17">
         <v>0</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1838,63 +1775,63 @@
         <v>0</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="G18" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H18">
-        <v>10.5</v>
+        <v>20.56</v>
       </c>
       <c r="I18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J18">
         <v>0</v>
       </c>
       <c r="K18">
-        <v>13.2</v>
+        <v>15.89</v>
       </c>
       <c r="L18">
-        <v>948.56</v>
+        <v>765.15</v>
       </c>
       <c r="M18">
-        <v>75.88</v>
+        <v>61.21</v>
       </c>
       <c r="N18">
-        <v>90.69</v>
+        <v>92.81</v>
       </c>
       <c r="O18">
-        <v>17.559999999999999</v>
+        <v>20.13</v>
       </c>
       <c r="P18">
-        <v>35.159999999999997</v>
+        <v>34.159999999999997</v>
       </c>
       <c r="Q18" t="s">
+        <v>18</v>
+      </c>
+      <c r="R18" t="s">
         <v>38</v>
       </c>
-      <c r="R18" t="s">
-        <v>58</v>
-      </c>
       <c r="S18">
         <v>0</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1903,63 +1840,63 @@
         <v>0</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="G19" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H19">
-        <v>20.56</v>
+        <v>22</v>
       </c>
       <c r="I19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19">
-        <v>15.89</v>
+        <v>11.45</v>
       </c>
       <c r="L19">
-        <v>765.15</v>
+        <v>455.98</v>
       </c>
       <c r="M19">
-        <v>61.21</v>
+        <v>36.479999999999997</v>
       </c>
       <c r="N19">
-        <v>92.81</v>
+        <v>63.61</v>
       </c>
       <c r="O19">
-        <v>20.13</v>
+        <v>21.95</v>
       </c>
       <c r="P19">
-        <v>34.159999999999997</v>
+        <v>32.130000000000003</v>
       </c>
       <c r="Q19" t="s">
+        <v>19</v>
+      </c>
+      <c r="R19" t="s">
         <v>39</v>
       </c>
-      <c r="R19" t="s">
-        <v>59</v>
-      </c>
       <c r="S19">
         <v>0</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1968,123 +1905,58 @@
         <v>0</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="G20" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H20">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20">
-        <v>11.45</v>
+        <v>10.26</v>
       </c>
       <c r="L20">
-        <v>455.98</v>
+        <v>987.65</v>
       </c>
       <c r="M20">
-        <v>36.479999999999997</v>
+        <v>79.010000000000005</v>
       </c>
       <c r="N20">
-        <v>63.61</v>
+        <v>140.54</v>
       </c>
       <c r="O20">
-        <v>21.95</v>
+        <v>22.23</v>
       </c>
       <c r="P20">
-        <v>32.130000000000003</v>
+        <v>42.98</v>
       </c>
       <c r="Q20" t="s">
+        <v>20</v>
+      </c>
+      <c r="R20" t="s">
         <v>40</v>
       </c>
-      <c r="R20" t="s">
-        <v>60</v>
-      </c>
       <c r="S20">
         <v>0</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G21" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21">
-        <v>23</v>
-      </c>
-      <c r="I21">
-        <v>5</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>10.26</v>
-      </c>
-      <c r="L21">
-        <v>987.65</v>
-      </c>
-      <c r="M21">
-        <v>79.010000000000005</v>
-      </c>
-      <c r="N21">
-        <v>140.54</v>
-      </c>
-      <c r="O21">
-        <v>22.23</v>
-      </c>
-      <c r="P21">
-        <v>42.98</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>41</v>
-      </c>
-      <c r="R21" t="s">
-        <v>61</v>
-      </c>
-      <c r="S21">
-        <v>0</v>
-      </c>
-      <c r="T21" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="U21" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>